<commit_message>
commit before pulling from main
</commit_message>
<xml_diff>
--- a/arian-scripts/Kubrick MI Diff.xlsx
+++ b/arian-scripts/Kubrick MI Diff.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ten10" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpartaGlobal" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -981,4 +982,2365 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AZ9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date of Collection</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Website_URL</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Public/Private</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Practices</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Practices_URL</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Services</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Services_URL</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Solutions</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Solutions_URL</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Previous Close</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>52 Week Range</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Sector</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Full Time Employees</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Fiscal Year Ends</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>EBITDA</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Company NPS</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Company Glassdoor</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>MI Summary</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Competitive Threat Level</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Market Share</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Pricing Strategy</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Target Market_1</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Target Market_2</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Channels-to-Market_1 (Social Media)</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Channels-to-Market_2 (Sales)</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Channels-to-Market_3 (Promotions/Sponsorship)</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Market Differentiation (USP)</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue Trends</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Profitability</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Growth Rate</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue per Employee</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Satisfaction</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Reviews &amp; Ratings</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Complaints</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Innovation</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Tech Advancements</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Patents &amp; Intellectual Property</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Emerging Trends</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Potential Threats</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Long-term Strategy</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Recent Activities</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Market Responsiveness</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Key Executives</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Company Culture</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Compliance Requirements</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Legal Issues/Pending Litigations</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Environmental Impact</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>Social Initiatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SpartaGlobal</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/careers/</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Business Analysis</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/our-services/business-analysis/</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SpartaGlobal</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/careers/</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Cybersecurity</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/our-services/cybersecurity/</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AR3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SpartaGlobal</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/careers/</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/our-services/data/</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AR4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AS4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AT4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AY4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AZ4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SpartaGlobal</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/careers/</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Devops</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/our-services/devops/</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AM5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AN5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AR5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AS5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AT5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AV5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AX5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AY5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AZ5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SpartaGlobal</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/careers/</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Manual Test</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/our-services/manual-test/</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AR6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AS6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AT6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AY6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AZ6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SpartaGlobal</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/careers/</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Project Management</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/our-services/project-management/</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AM7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AN7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AO7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AP7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AQ7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AR7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AS7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AT7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AU7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AV7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AW7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AX7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AY7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AZ7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SpartaGlobal</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/careers/</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/our-services/software-development/</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AL8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AM8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AN8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AO8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AP8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AQ8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AR8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AS8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AT8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AU8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AV8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AW8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AX8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AY8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AZ8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SpartaGlobal</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/careers/</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Test Engineering</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://www.spartaglobal.com/our-services/test-engineering/</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AM9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AN9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AO9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AP9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AQ9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AR9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AS9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AT9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AU9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AV9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AW9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AX9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AY9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="AZ9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>